<commit_message>
finished comand summary spreadsheet
</commit_message>
<xml_diff>
--- a/Command Classifications.xlsx
+++ b/Command Classifications.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="63">
   <si>
     <t>&lt;&lt;&lt;&lt;&lt;&lt;Simple Commands&gt;&gt;&gt;&gt;&gt;&gt;</t>
   </si>
@@ -22,9 +22,6 @@
     <t>&lt;&lt;&lt;&lt;&lt;&lt;&lt;Complex Commands&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;</t>
   </si>
   <si>
-    <t>keyword and zero parameters</t>
-  </si>
-  <si>
     <t>Keyword + parameter</t>
   </si>
   <si>
@@ -164,6 +161,48 @@
   </si>
   <si>
     <t>Command trees execute in post order</t>
+  </si>
+  <si>
+    <t>FORWARD val1</t>
+  </si>
+  <si>
+    <t>BACK val1</t>
+  </si>
+  <si>
+    <t>LEFT val1</t>
+  </si>
+  <si>
+    <t>RIGHT val1</t>
+  </si>
+  <si>
+    <t>SETHEADING val1</t>
+  </si>
+  <si>
+    <t>TOWARDS val1 val2</t>
+  </si>
+  <si>
+    <t>SETXY val1 val2</t>
+  </si>
+  <si>
+    <t>PENDOWN</t>
+  </si>
+  <si>
+    <t>PENUP</t>
+  </si>
+  <si>
+    <t>SHOWTURTLE</t>
+  </si>
+  <si>
+    <t>HIDETURTLE</t>
+  </si>
+  <si>
+    <t>HOME</t>
+  </si>
+  <si>
+    <t>CLEARSCREEN</t>
+  </si>
+  <si>
+    <t>keyword + zero parameters</t>
   </si>
 </sst>
 </file>
@@ -806,7 +845,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
@@ -857,6 +896,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1199,10 +1241,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1226,77 +1268,77 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>3</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>4</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="C3" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="E3" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="F3" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="G3" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="H3" s="19" t="s">
         <v>14</v>
-      </c>
-      <c r="H3" s="19" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="13" t="s">
         <v>17</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>18</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G4" s="8"/>
       <c r="H4" s="6"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="C5" s="13" t="s">
         <v>21</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>22</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="5"/>
@@ -1305,11 +1347,13 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="13" t="s">
         <v>23</v>
-      </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="13" t="s">
-        <v>24</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="8"/>
@@ -1318,11 +1362,13 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="13" t="s">
         <v>25</v>
-      </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="13" t="s">
-        <v>26</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="10"/>
@@ -1330,117 +1376,149 @@
       <c r="H7" s="11"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8"/>
+      <c r="A8" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>51</v>
+      </c>
       <c r="C8" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="13" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="13" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="13" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="13" t="s">
-        <v>29</v>
-      </c>
-    </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
+      <c r="A11" s="12" t="s">
+        <v>19</v>
+      </c>
       <c r="B11" s="8"/>
       <c r="C11" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
+      <c r="A12" s="12" t="s">
+        <v>22</v>
+      </c>
       <c r="B12" s="8"/>
       <c r="C12" s="13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="7"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="9"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="14" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="14" t="s">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="26" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E14" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="26" t="s">
+      <c r="B17" s="1"/>
+      <c r="C17" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="26" t="s">
+      <c r="E17" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="E15" s="22" t="s">
+      <c r="C18" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" s="20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F19" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F20" s="20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C21" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="E21" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="F15" s="23" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="F16" s="20" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="F17" s="20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F18" s="20" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C19" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F19" s="21">
+      <c r="F21" s="21">
         <v>1</v>
       </c>
     </row>

</xml_diff>